<commit_message>
fix readxls overcounting sim count
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/MaxsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/MaxsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AA9762-41FA-4937-80EE-22AD7ABB0045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC681824-D2AE-4C65-A2AA-0B56E9AD3495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -720,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:AC84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>7200</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -860,12 +860,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -876,7 +876,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -887,7 +887,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -898,7 +898,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -909,26 +909,27 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="2">
         <v>0.01</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -939,21 +940,22 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="2">
         <v>1E-4</v>
       </c>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -964,21 +966,22 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="2">
         <v>0.01</v>
       </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -989,7 +992,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1030,15 +1033,15 @@
         <v>49</v>
       </c>
       <c r="C36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" t="s">
         <v>52</v>
@@ -1046,14 +1049,15 @@
       <c r="C38" s="2">
         <v>9.9999999999999991E-22</v>
       </c>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>54</v>
       </c>
@@ -1061,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -1072,12 +1076,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>22</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -1121,7 +1125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>-0.52359877559829882</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1145,7 +1149,7 @@
         <v>0.52359877559829882</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -1157,7 +1161,7 @@
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>69</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>-1.8429999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>70</v>
       </c>
@@ -1173,7 +1177,7 @@
         <v>0.37819999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>71</v>
       </c>
@@ -1182,7 +1186,7 @@
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -1193,12 +1197,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>73</v>
       </c>
@@ -1206,7 +1210,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>75</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>77</v>
       </c>
@@ -1222,7 +1226,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -1233,16 +1237,17 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>82</v>
       </c>
       <c r="C61" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="AB61" s="4"/>
+      <c r="AC61" s="4"/>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>83</v>
       </c>
@@ -1250,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>84</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
agentcontrol overhaul and more
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/MaxsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/MaxsLaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC681824-D2AE-4C65-A2AA-0B56E9AD3495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A9D48C-1596-4F30-8114-10A6C06B5452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3696" yWindow="828" windowWidth="16080" windowHeight="10896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
   <si>
     <t>dt</t>
   </si>
@@ -385,6 +385,15 @@
   </si>
   <si>
     <t>findNeighborhood_KNNInFixedRadius</t>
+  </si>
+  <si>
+    <t>followRadius</t>
+  </si>
+  <si>
+    <t>Frames to skip between Neighborhood Updates</t>
+  </si>
+  <si>
+    <t>neighborFrameSkip</t>
   </si>
 </sst>
 </file>
@@ -720,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC84"/>
+  <dimension ref="A1:AC86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>72</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -778,7 +787,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>60</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -822,31 +831,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>2600</v>
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -854,264 +863,264 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>9.81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0.01</v>
       </c>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1E-4</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0.01</v>
       </c>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
       <c r="B32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32">
-        <v>-3</v>
+        <v>40</v>
+      </c>
+      <c r="C32" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>50</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>49</v>
       </c>
-      <c r="C36">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="C37">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="2">
-        <v>9.9999999999999991E-22</v>
       </c>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="1"/>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="2">
+        <v>9.9999999999999991E-22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>54</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>55</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44">
-        <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
@@ -1119,22 +1128,21 @@
         <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48">
-        <f>-2/12*PI()</f>
-        <v>-0.52359877559829882</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
@@ -1142,300 +1150,320 @@
         <v>65</v>
       </c>
       <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49">
+        <f>-2/12*PI()</f>
+        <v>-0.52359877559829882</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
         <v>66</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <f>2/12*PI()</f>
         <v>0.52359877559829882</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>68</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>67</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <f>11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51">
-        <v>-1.8429999999999998E-2</v>
-      </c>
-    </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52">
-        <v>0.37819999999999998</v>
+        <v>-1.8429999999999998E-2</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
         <v>71</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <f>-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>15</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>111</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
         <v>77</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>81</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>79</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" s="4" t="b">
-        <v>1</v>
       </c>
       <c r="AB61" s="4"/>
       <c r="AC61" s="4"/>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" t="b">
+        <v>82</v>
+      </c>
+      <c r="C62" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>87</v>
       </c>
-      <c r="C66" t="b">
+      <c r="C67" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="B68" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>89</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
         <v>91</v>
       </c>
-      <c r="C70">
+      <c r="C72">
         <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" t="s">
-        <v>92</v>
-      </c>
-      <c r="C71">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" t="s">
-        <v>93</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C74">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C75">
-        <v>800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="B76" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>500</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C77">
-        <v>10</v>
+        <v>800</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C78">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C79">
-        <v>2000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>104</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>101</v>
       </c>
-      <c r="C80">
+      <c r="C82">
         <v>4000</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
         <v>108</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
         <v>109</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
slight adjustment to coloring
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/MaxsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/MaxsLaw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxlg\Dropbox (ASU)\PC\Documents\GitHub\REU_MatlabSim\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A9D48C-1596-4F30-8114-10A6C06B5452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97855E98-D2BD-464F-A952-91648054957F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="828" windowWidth="16080" windowHeight="10896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="122">
   <si>
     <t>dt</t>
   </si>
@@ -276,9 +276,6 @@
     <t>renderScale</t>
   </si>
   <si>
-    <t>[150;150]</t>
-  </si>
-  <si>
     <t>[scaleX,scaleY]</t>
   </si>
   <si>
@@ -394,6 +391,15 @@
   </si>
   <si>
     <t>neighborFrameSkip</t>
+  </si>
+  <si>
+    <t>[100;100]</t>
+  </si>
+  <si>
+    <t>Multiplier to intensify bank angle based on thermal strength</t>
+  </si>
+  <si>
+    <t>thermalBankFactor</t>
   </si>
 </sst>
 </file>
@@ -729,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC86"/>
+  <dimension ref="A1:AC87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,7 +752,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -787,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -825,7 +831,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -833,10 +839,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
         <v>118</v>
-      </c>
-      <c r="B11" t="s">
-        <v>119</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -855,7 +861,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,7 +899,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
@@ -972,7 +978,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="2">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
@@ -998,7 +1004,7 @@
         <v>40</v>
       </c>
       <c r="C32" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
@@ -1053,7 +1059,7 @@
         <v>49</v>
       </c>
       <c r="C37">
-        <v>100000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
@@ -1211,81 +1217,84 @@
         <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
         <v>77</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" t="s">
         <v>79</v>
       </c>
-      <c r="C61" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB61" s="4"/>
-      <c r="AC61" s="4"/>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="C62" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB62" s="4"/>
+      <c r="AC62" s="4"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" t="b">
+        <v>81</v>
+      </c>
+      <c r="C63" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -1293,7 +1302,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -1301,47 +1310,44 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="C68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69">
+        <v>1500</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
-        <v>89</v>
-      </c>
-      <c r="C71" t="s">
-        <v>90</v>
+      <c r="A71" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72">
-        <v>50</v>
+        <v>88</v>
+      </c>
+      <c r="C72" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>102</v>
-      </c>
       <c r="B73" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C73">
         <v>50</v>
@@ -1349,13 +1355,13 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1363,7 +1369,7 @@
         <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1371,13 +1377,13 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C76">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1385,32 +1391,32 @@
         <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C77">
-        <v>800</v>
+        <v>500</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>800</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C79">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1418,53 +1424,64 @@
         <v>105</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C80">
-        <v>1E-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C81">
-        <v>2000</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C82">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C83">
         <v>4000</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B85" t="s">
-        <v>108</v>
-      </c>
-      <c r="C85" t="s">
-        <v>115</v>
+      <c r="A85" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C86" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>